<commit_message>
draw lines working, doesnt seem exactly right for test/filter_edge_color/5
</commit_message>
<xml_diff>
--- a/test/filter_edge_color/5/draw_line.xlsx
+++ b/test/filter_edge_color/5/draw_line.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kushn\projects\cv-workbench\test\filter_edge_color\5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74769AE0-D981-4E41-A974-DCFC66934618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5E4176-F57A-4E92-8603-14E9C33957F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2424" yWindow="1584" windowWidth="17232" windowHeight="8880" xr2:uid="{2BCE48CD-1D07-4A04-8A32-503AC9A36AB7}"/>
+    <workbookView xWindow="-25980" yWindow="4005" windowWidth="21750" windowHeight="10590" xr2:uid="{2BCE48CD-1D07-4A04-8A32-503AC9A36AB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>theta</t>
   </si>
@@ -54,6 +54,18 @@
   </si>
   <si>
     <t>rho</t>
+  </si>
+  <si>
+    <t>x_min</t>
+  </si>
+  <si>
+    <t>x_max</t>
+  </si>
+  <si>
+    <t>y_min</t>
+  </si>
+  <si>
+    <t>y_max</t>
   </si>
 </sst>
 </file>
@@ -69,12 +81,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -89,8 +113,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,147 +453,196 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19DACBE5-68B9-4970-9676-AD7DF721B2B8}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
+        <v>-32</v>
+      </c>
+      <c r="B2">
         <v>84</v>
       </c>
-      <c r="B2">
-        <f>COS($A$2*3.1416/180)</f>
+      <c r="C2" s="2">
+        <f>COS($B2*3.1416/180)</f>
         <v>0.10452505372299775</v>
       </c>
-      <c r="C2">
-        <f>SIN($A$2*3.1416/180)</f>
+      <c r="D2" s="2">
+        <f>SIN($B2*3.1416/180)</f>
         <v>0.99452225371994796</v>
       </c>
-      <c r="D2">
+      <c r="E2" s="3">
         <v>-159.5</v>
       </c>
-      <c r="E2">
-        <v>-32</v>
-      </c>
-      <c r="F2">
-        <f>(D2*B2-E2)/C2</f>
+      <c r="F2" s="4">
+        <f>(E2*$C2-$A2)/$D2</f>
         <v>15.412680685472335</v>
       </c>
+      <c r="G2" s="3">
+        <v>159.5</v>
+      </c>
+      <c r="H2" s="4">
+        <f>(G2*$C2-$A2)/$D2</f>
+        <v>48.939826018738678</v>
+      </c>
+      <c r="I2" s="3">
+        <v>-119.5</v>
+      </c>
+      <c r="J2" s="2">
+        <f>($A2-I2*$D2)/$C2</f>
+        <v>830.85735167075961</v>
+      </c>
+      <c r="K2" s="3">
+        <v>119.5</v>
+      </c>
+      <c r="L2" s="2">
+        <f>($A2-K2*$D2)/$C2</f>
+        <v>-1443.1507466075052</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>84</v>
+        <v>-76</v>
       </c>
       <c r="B3">
-        <f>COS($A$2*3.1416/180)</f>
-        <v>0.10452505372299775</v>
-      </c>
-      <c r="C3">
-        <f>SIN($A$2*3.1416/180)</f>
-        <v>0.99452225371994796</v>
-      </c>
-      <c r="D3">
+        <v>81</v>
+      </c>
+      <c r="C3" s="2">
+        <f t="shared" ref="C3:C4" si="0">COS($B3*3.1416/180)</f>
+        <v>0.15643119985570828</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" ref="D3:D4" si="1">SIN($B3*3.1416/180)</f>
+        <v>0.98768885774402837</v>
+      </c>
+      <c r="E3" s="3">
+        <f>E2</f>
+        <v>-159.5</v>
+      </c>
+      <c r="F3" s="4">
+        <f>(E3*$C3-$A3)/$D3</f>
+        <v>51.685531554558203</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G4" si="2">G2</f>
         <v>159.5</v>
       </c>
-      <c r="E3">
-        <v>-32</v>
-      </c>
-      <c r="F3">
-        <f>(D3*B3-E3)/C3</f>
-        <v>48.939826018738678</v>
+      <c r="H3" s="4">
+        <f>(G3*$C3-$A3)/$D3</f>
+        <v>102.20908698673212</v>
+      </c>
+      <c r="I3" s="3">
+        <f t="shared" ref="I3:I4" si="3">I2</f>
+        <v>-119.5</v>
+      </c>
+      <c r="J3" s="2">
+        <f>($A3-I3*$D3)/$C3</f>
+        <v>268.67286410369962</v>
+      </c>
+      <c r="K3" s="3">
+        <f t="shared" ref="K3:K4" si="4">K2</f>
+        <v>119.5</v>
+      </c>
+      <c r="L3" s="2">
+        <f>($A3-K3*$D3)/$C3</f>
+        <v>-1240.3460350581154</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B6" si="0">COS($A$2*3.1416/180)</f>
-        <v>0.10452505372299775</v>
-      </c>
-      <c r="C4">
-        <f t="shared" ref="C4:C6" si="1">SIN($A$2*3.1416/180)</f>
-        <v>0.99452225371994796</v>
-      </c>
-      <c r="D4">
-        <f>(E4-F4*C4)/B4</f>
-        <v>830.85735167075961</v>
-      </c>
-      <c r="E4">
-        <v>-32</v>
-      </c>
-      <c r="F4">
+        <v>93</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" si="0"/>
+        <v>-5.2339746686040321E-2</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99862933609865534</v>
+      </c>
+      <c r="E4" s="3">
+        <f>E3</f>
+        <v>-159.5</v>
+      </c>
+      <c r="F4" s="4">
+        <f>(E4*$C4-$A4)/$D4</f>
+        <v>-11.667803040011512</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="2"/>
+        <v>159.5</v>
+      </c>
+      <c r="H4" s="4">
+        <f>(G4*$C4-$A4)/$D4</f>
+        <v>-28.387098767968592</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" si="3"/>
         <v>-119.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>84</v>
-      </c>
-      <c r="B5">
-        <f t="shared" si="0"/>
-        <v>0.10452505372299775</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="1"/>
-        <v>0.99452225371994796</v>
-      </c>
-      <c r="D5">
-        <f>(E5-F5*C5)/B5</f>
-        <v>-1443.1507466075052</v>
-      </c>
-      <c r="E5">
-        <v>-32</v>
-      </c>
-      <c r="F5">
+      <c r="J4" s="2">
+        <f>($A4-I4*$D4)/$C4</f>
+        <v>-2662.1490260470073</v>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" si="4"/>
         <v>119.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>81</v>
-      </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>0.10452505372299775</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="1"/>
-        <v>0.99452225371994796</v>
-      </c>
-      <c r="D6">
-        <f>(E6-F6*C6)/B6</f>
-        <v>-1864.1024556265177</v>
-      </c>
-      <c r="E6">
-        <v>-76</v>
-      </c>
-      <c r="F6">
-        <v>119.5</v>
+      <c r="L4" s="2">
+        <f>($A4-K4*$D4)/$C4</f>
+        <v>1897.9114717474081</v>
       </c>
     </row>
   </sheetData>

</xml_diff>